<commit_message>
Game Update and Audio Assets
Pushing the most recent version of the game as well as the audio samples I have downloaded and recorded.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Spring 2021\Production Studio\Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Spring 2021\Production Studio\Project Repo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A69D510-6D67-4300-B27A-19F135F8F30D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E28E024-3F67-4F2F-855D-3E26A1059940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -672,12 +672,16 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="52" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
FMOD events and some Unity audio
Created all the fmod events and started implementing some of the sound effects in Unity.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitch\Desktop\School\Spring 2021\Production Studio\Survive or Die Trying Repo\Survive-or-Die-Trying\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93393829-2E6C-4844-AA06-20A690CA29F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6FFB36-8B6E-421A-A500-95A74BDE4556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>Drink Water</t>
   </si>
   <si>
-    <t>Not Done</t>
-  </si>
-  <si>
     <t>Dialog</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>trees groaning, wind</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,16 +709,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,16 +726,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,16 +743,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -760,16 +760,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -777,16 +777,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -794,16 +794,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,16 +811,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,33 +828,33 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
         <v>69</v>
       </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -862,16 +862,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -879,50 +879,50 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,16 +930,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,16 +947,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,16 +964,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,16 +981,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,16 +998,16 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,16 +1015,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,16 +1032,16 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1049,16 +1049,16 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,186 +1066,186 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
         <v>98</v>
       </c>
-      <c r="C33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
-      </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing more audio in the game
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Spring 2021\Production Studio\Project Repo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4807F9-EBD3-42C1-BE37-1DAC34E298E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160B9FF7-335C-4599-9D18-B1D857160F47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="104">
   <si>
     <t>Event Name</t>
   </si>
@@ -333,10 +333,10 @@
     <t>trees groaning, wind</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>DUE</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -885,6 +885,9 @@
       <c r="E11" t="s">
         <v>100</v>
       </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -902,6 +905,9 @@
       <c r="E12" t="s">
         <v>100</v>
       </c>
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -917,9 +923,6 @@
         <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -939,6 +942,9 @@
       <c r="E14" t="s">
         <v>100</v>
       </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -974,7 +980,7 @@
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -994,7 +1000,7 @@
         <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,7 +1020,7 @@
         <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,7 +1037,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,7 +1054,7 @@
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,9 +1071,6 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1085,9 +1088,6 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1105,9 +1105,6 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1128,7 +1125,7 @@
         <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1148,7 +1145,7 @@
         <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1165,9 +1162,6 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1188,7 +1182,7 @@
         <v>100</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,10 +1199,10 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,9 +1221,6 @@
       <c r="E29" t="s">
         <v>100</v>
       </c>
-      <c r="F29" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1247,9 +1238,6 @@
       <c r="E30" t="s">
         <v>100</v>
       </c>
-      <c r="F30" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1265,7 +1253,7 @@
         <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,13 +1270,10 @@
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
@@ -1303,9 +1288,6 @@
       </c>
       <c r="E33" t="s">
         <v>100</v>
-      </c>
-      <c r="F33" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polishing ambience and adding some more sound effects to the game
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Spring 2021\Production Studio\Project Repo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160B9FF7-335C-4599-9D18-B1D857160F47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFFCB81-2A67-418F-911F-E33A548446F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="104">
   <si>
     <t>Event Name</t>
   </si>
@@ -237,12 +237,6 @@
     <t>swinging the axe and hitting a surface that is not a tree</t>
   </si>
   <si>
-    <t>bear growling before attacking</t>
-  </si>
-  <si>
-    <t>bear roaring when idling or attacking</t>
-  </si>
-  <si>
     <t>leaves rustling in the wind, trees groaning in wind, ambient forest sound</t>
   </si>
   <si>
@@ -333,10 +327,16 @@
     <t>trees groaning, wind</t>
   </si>
   <si>
-    <t>DUE</t>
-  </si>
-  <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>bear roaring when attacking</t>
+  </si>
+  <si>
+    <t>bear growling when idling</t>
+  </si>
+  <si>
+    <t>FIXING BUGS</t>
   </si>
 </sst>
 </file>
@@ -675,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,10 +687,10 @@
     <col min="2" max="2" width="72" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -707,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -721,10 +721,10 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -738,10 +738,10 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -755,15 +755,15 @@
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
@@ -772,18 +772,15 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -792,38 +789,32 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -832,15 +823,15 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -849,10 +840,10 @@
         <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -866,15 +857,15 @@
         <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -883,18 +874,15 @@
         <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -903,35 +891,32 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
@@ -942,16 +927,13 @@
       <c r="E14" t="s">
         <v>100</v>
       </c>
-      <c r="F14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -960,15 +942,15 @@
         <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -977,18 +959,15 @@
         <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -997,18 +976,15 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
@@ -1017,18 +993,15 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -1037,15 +1010,15 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1054,15 +1027,15 @@
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -1071,15 +1044,15 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -1088,15 +1061,15 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
@@ -1105,15 +1078,15 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -1122,18 +1095,15 @@
         <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -1142,18 +1112,15 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -1162,15 +1129,15 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -1179,18 +1146,15 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -1199,18 +1163,15 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1219,15 +1180,15 @@
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -1236,15 +1197,15 @@
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -1253,15 +1214,15 @@
         <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1270,7 +1231,7 @@
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,16 +1239,16 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
         <v>39</v>
       </c>
       <c r="D33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" t="s">
         <v>98</v>
-      </c>
-      <c r="E33" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some game work, bug fixes, and adding some more audio into the game
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Spring 2021\Production Studio\Project Repo\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitch\Desktop\School\Spring 2021\Production Studio\Survive or Die Trying Repo\Survive-or-Die-Trying\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFFCB81-2A67-418F-911F-E33A548446F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0612BBE2-D6A2-41FA-8770-25A0BDBF6488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding the last audio events into the game.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitch\Desktop\School\Spring 2021\Production Studio\Survive or Die Trying Repo\Survive-or-Die-Trying\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0612BBE2-D6A2-41FA-8770-25A0BDBF6488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E0060-614A-4138-B841-D00517D8FE83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="103">
   <si>
     <t>Event Name</t>
   </si>
@@ -321,9 +321,6 @@
     <t>swimming loop</t>
   </si>
   <si>
-    <t>Made</t>
-  </si>
-  <si>
     <t>trees groaning, wind</t>
   </si>
   <si>
@@ -336,7 +333,7 @@
     <t>bear growling when idling</t>
   </si>
   <si>
-    <t>FIXING BUGS</t>
+    <t>POSTPONED (Feature not in game yet)</t>
   </si>
 </sst>
 </file>
@@ -677,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +684,7 @@
     <col min="2" max="2" width="72" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -721,7 +718,7 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -738,7 +735,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -755,7 +752,7 @@
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,7 +769,7 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,7 +786,7 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -806,7 +803,7 @@
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,7 +820,7 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,7 +837,7 @@
         <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
         <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,7 +862,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -874,7 +871,7 @@
         <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -882,7 +879,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -891,7 +888,7 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,10 +902,10 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -925,7 +922,7 @@
         <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -942,7 +939,7 @@
         <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,7 +956,7 @@
         <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -976,7 +973,7 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,7 +990,7 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1010,7 +1007,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1027,7 +1024,7 @@
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,7 +1041,7 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1061,7 +1058,7 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,7 +1075,7 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,7 +1092,7 @@
         <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1112,7 +1109,7 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,7 +1126,7 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,7 +1143,7 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,7 +1160,7 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,7 +1177,7 @@
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,7 +1194,7 @@
         <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,7 +1211,7 @@
         <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,7 +1228,7 @@
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,7 +1245,7 @@
         <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>